<commit_message>
More test results added
</commit_message>
<xml_diff>
--- a/test/private_template_scheme/private_template_scheme.xlsx
+++ b/test/private_template_scheme/private_template_scheme.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andrea\Desktop\Main\City\Individual Project\Source code\test\private_template_scheme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB3B1CA-8285-4F5F-A820-C225E828E6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565E8554-8A45-4309-84DA-95BF3DA8E697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8010" yWindow="1770" windowWidth="16065" windowHeight="15510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>nsym</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>8x512</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>Notes</t>
@@ -574,7 +571,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>1</v>
@@ -617,10 +614,10 @@
         <v>3</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -631,10 +628,10 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="16" t="s">
         <v>15</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -655,11 +652,11 @@
         <f xml:space="preserve"> (5 * SUM(1, -E4) + 4 * SUM(1, -D4)) / 9</f>
         <v>0.59622222222222221</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>12</v>
+      <c r="G4" s="12">
+        <v>0.81043026203594604</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0.76421047685188404</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -678,11 +675,11 @@
         <f t="shared" ref="F5:F36" si="0" xml:space="preserve"> (5 * SUM(1, -E5) + 4 * SUM(1, -D5)) / 9</f>
         <v>0.6283333333333333</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>12</v>
+      <c r="G5" s="12">
+        <v>0.82003114073988903</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0.77763542662011798</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -701,11 +698,11 @@
         <f t="shared" si="0"/>
         <v>0.65794444444444444</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>12</v>
+      <c r="G6" s="12">
+        <v>0.81355305833292502</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0.79161999328722099</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -724,11 +721,11 @@
         <f t="shared" si="0"/>
         <v>0.75566666666666671</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>12</v>
+      <c r="G7" s="12">
+        <v>0.81045561990773995</v>
+      </c>
+      <c r="H7" s="12">
+        <v>1.21965424699037</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -747,11 +744,11 @@
         <f t="shared" si="0"/>
         <v>0.8382222222222222</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>12</v>
+      <c r="G8" s="12">
+        <v>0.82076074074144201</v>
+      </c>
+      <c r="H8" s="12">
+        <v>1.1777451317129</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -782,11 +779,11 @@
         <f t="shared" si="0"/>
         <v>0.44444444444444442</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>12</v>
+      <c r="G10" s="12">
+        <v>0.95126683101860998</v>
+      </c>
+      <c r="H10" s="12">
+        <v>0.95695051331029002</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -805,11 +802,11 @@
         <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>12</v>
+      <c r="G11" s="12">
+        <v>0.85050280786957999</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0.85439606678242996</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -828,11 +825,11 @@
         <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="G12" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>12</v>
+      <c r="G12" s="12">
+        <v>0.84856873194446003</v>
+      </c>
+      <c r="H12" s="12">
+        <v>0.83986160964504997</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -851,11 +848,11 @@
         <f t="shared" si="0"/>
         <v>0.70166666666666666</v>
       </c>
-      <c r="G13" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>12</v>
+      <c r="G13" s="12">
+        <v>0.82575110786981998</v>
+      </c>
+      <c r="H13" s="12">
+        <v>0.84928780297082995</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -874,11 +871,11 @@
         <f t="shared" si="0"/>
         <v>0.716088888888889</v>
       </c>
-      <c r="G14" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>12</v>
+      <c r="G14" s="12">
+        <v>0.75164423888894005</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0.76165194814818005</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -897,11 +894,11 @@
         <f t="shared" si="0"/>
         <v>0.76287777777777777</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>12</v>
+      <c r="G15" s="12">
+        <v>0.73949590138889998</v>
+      </c>
+      <c r="H15" s="12">
+        <v>0.76850170108025995</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -911,20 +908,20 @@
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="3">
-        <v>0</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="E16" s="3">
         <v>0.36109999999999998</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="0"/>
-        <v>0.79938888888888882</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>12</v>
+        <v>0.79627777777777775</v>
+      </c>
+      <c r="G16" s="12">
+        <v>0.77620039629631998</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0.79764093827159999</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -943,11 +940,11 @@
         <f t="shared" si="0"/>
         <v>0.84363333333333346</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>12</v>
+      <c r="G17" s="12">
+        <v>0.83138462037036998</v>
+      </c>
+      <c r="H17" s="12">
+        <v>0.88626506284721995</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -966,11 +963,11 @@
         <f t="shared" si="0"/>
         <v>0.86655555555555552</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>12</v>
+      <c r="G18" s="12">
+        <v>0.75948153888889003</v>
+      </c>
+      <c r="H18" s="12">
+        <v>0.80326767939815003</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -989,11 +986,11 @@
         <f t="shared" si="0"/>
         <v>0.87197777777777774</v>
       </c>
-      <c r="G19" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>12</v>
+      <c r="G19" s="12">
+        <v>0.77042453564815006</v>
+      </c>
+      <c r="H19" s="12">
+        <v>0.81885725563272005</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1024,11 +1021,11 @@
         <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="G21" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>12</v>
+      <c r="G21" s="12">
+        <v>0.76798957407326796</v>
+      </c>
+      <c r="H21" s="12">
+        <v>0.76836267453731</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1047,11 +1044,11 @@
         <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="G22" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>12</v>
+      <c r="G22" s="12">
+        <v>0.73466754259277001</v>
+      </c>
+      <c r="H22" s="12">
+        <v>0.73380146296325199</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1070,11 +1067,11 @@
         <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="G23" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>12</v>
+      <c r="G23" s="12">
+        <v>0.72888866666714103</v>
+      </c>
+      <c r="H23" s="12">
+        <v>0.73438412885805504</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1093,11 +1090,11 @@
         <f t="shared" si="0"/>
         <v>0.79397777777777767</v>
       </c>
-      <c r="G24" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>12</v>
+      <c r="G24" s="12">
+        <v>0.73145039907346099</v>
+      </c>
+      <c r="H24" s="12">
+        <v>0.76064012407411496</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1116,11 +1113,11 @@
         <f t="shared" si="0"/>
         <v>0.81413333333333326</v>
       </c>
-      <c r="G25" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>12</v>
+      <c r="G25" s="12">
+        <v>0.74139222777833902</v>
+      </c>
+      <c r="H25" s="12">
+        <v>0.77248586049391099</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1151,11 +1148,11 @@
         <f t="shared" si="0"/>
         <v>0.70175555555555547</v>
       </c>
-      <c r="G27" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>12</v>
+      <c r="G27" s="12">
+        <v>0.78071386851715197</v>
+      </c>
+      <c r="H27" s="12">
+        <v>0.75688793773109897</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1164,10 +1161,7 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
-      <c r="F28" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="F28" s="3"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
     </row>
@@ -1175,7 +1169,9 @@
       <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="5"/>
+      <c r="B29" s="5">
+        <v>159</v>
+      </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5">
         <v>1.6199999999999999E-2</v>
@@ -1187,11 +1183,11 @@
         <f t="shared" si="0"/>
         <v>0.70602222222222233</v>
       </c>
-      <c r="G29" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="12" t="s">
-        <v>12</v>
+      <c r="G29" s="12">
+        <v>0.781758357407347</v>
+      </c>
+      <c r="H29" s="12">
+        <v>0.78634217476849599</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1222,11 +1218,11 @@
         <f t="shared" si="0"/>
         <v>0.66561111111111115</v>
       </c>
-      <c r="G31" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="12" t="s">
-        <v>12</v>
+      <c r="G31" s="12">
+        <v>0.79467081111134596</v>
+      </c>
+      <c r="H31" s="12">
+        <v>0.79921258194425904</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1245,11 +1241,11 @@
         <f t="shared" si="0"/>
         <v>0.70805555555555566</v>
       </c>
-      <c r="G32" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>12</v>
+      <c r="G32" s="12">
+        <v>0.80448897314784396</v>
+      </c>
+      <c r="H32" s="12">
+        <v>0.79895860833393095</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1268,11 +1264,11 @@
         <f t="shared" si="0"/>
         <v>0.73638888888888898</v>
       </c>
-      <c r="G33" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" s="12" t="s">
-        <v>12</v>
+      <c r="G33" s="12">
+        <v>0.78919971018573598</v>
+      </c>
+      <c r="H33" s="12">
+        <v>0.80330205740715899</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1291,11 +1287,11 @@
         <f t="shared" si="0"/>
         <v>0.81095555555555565</v>
       </c>
-      <c r="G34" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" s="12" t="s">
-        <v>12</v>
+      <c r="G34" s="12">
+        <v>0.89084253055625595</v>
+      </c>
+      <c r="H34" s="12">
+        <v>0.93885007314767899</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1314,11 +1310,11 @@
         <f t="shared" si="0"/>
         <v>0.84696666666666665</v>
       </c>
-      <c r="G35" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="12" t="s">
-        <v>12</v>
+      <c r="G35" s="12">
+        <v>0.81282625092663396</v>
+      </c>
+      <c r="H35" s="12">
+        <v>0.79424108657460402</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1337,11 +1333,11 @@
         <f t="shared" si="0"/>
         <v>0.78110000000000002</v>
       </c>
-      <c r="G36" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" s="12" t="s">
-        <v>12</v>
+      <c r="G36" s="12">
+        <v>0.79415257962709396</v>
+      </c>
+      <c r="H36" s="12">
+        <v>0.91232915046283602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>